<commit_message>
🔧 Zprovoznění tlačítek editace a archivace ve vyhledávání
- Napojení na existující modály (GitterboxModal, ItemModal, ArchiveModal)
- Oprava názvů metod (openEdit, openCreate místo openForEdit)
- Cache invalidation při refresh
- Všechna tlačítka nyní plně funkční
</commit_message>
<xml_diff>
--- a/backend/docs/vyskladneno_archiv.xlsx
+++ b/backend/docs/vyskladneno_archiv.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,12 +524,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-08-06</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14:44:36</t>
+          <t>10:56:20</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -543,29 +543,29 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>KOMPLETNÍ GB #23</t>
+          <t>KOMPLETNÍ GB #7</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2 položek</t>
+          <t>0 položek</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Rozbito/Poškozeno</t>
+          <t>Chyba/Špatně zaskladněno</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Částečně naplněný GB - kritická expirace! | uvolňuji místo, díly není třeba</t>
+          <t>........... | blbě zadaná data</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -575,7 +575,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Petr Dvořák</t>
+          <t>CCCCCCCC</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Položka_z_GB</t>
+          <t>Celý_GB</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -605,38 +605,30 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Mechanický díl</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>EU-SVA-156707-25</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Projekt Alpha</t>
-        </is>
-      </c>
+          <t>KOMPLETNÍ GB #23</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>13 ks</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>2026-05-14</t>
-        </is>
-      </c>
+          <t>2 položek</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
           <t>Rozbito/Poškozeno</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Částečně naplněný GB - kritická expirace! | uvolňuji místo, díly není třeba</t>
+        </is>
+      </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2025-05-14</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -671,12 +663,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Elektronická část</t>
+          <t>Mechanický díl</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>EU-SVA-471870-25</t>
+          <t>EU-SVA-156707-25</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -686,12 +678,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>26 ks</t>
+          <t>13 ks</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-05-14</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -699,14 +691,10 @@
           <t>Rozbito/Poškozeno</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Test položka 3</t>
-        </is>
-      </c>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2025-02-17</t>
+          <t>2025-05-14</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -723,7 +711,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>14:42:39</t>
+          <t>14:44:36</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -733,43 +721,55 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Celý_GB</t>
+          <t>Položka_z_GB</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>KOMPLETNÍ GB #15</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+          <t>Elektronická část</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>EU-SVA-471870-25</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Projekt Alpha</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0 položek</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
+          <t>26 ks</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Jiné</t>
+          <t>Rozbito/Poškozeno</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>....</t>
+          <t>Test položka 3</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-02-17</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Cibulka</t>
+          <t>Petr Dvořák</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>14:41:53</t>
+          <t>14:42:39</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Položka</t>
+          <t>Celý_GB</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -799,42 +799,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>topplate</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>EU-SVA-123456-25</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>STV</t>
-        </is>
-      </c>
+          <t>KOMPLETNÍ GB #15</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>10 ks</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>2025-08-01</t>
-        </is>
-      </c>
+          <t>0 položek</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Expirace</t>
+          <t>Jiné</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>cavity 2 | ttttttttttt</t>
+          <t>....</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -851,7 +839,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>14:34:25</t>
+          <t>14:41:53</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -865,26 +853,26 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Prototyp</t>
+          <t>topplate</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>EU-SVA-761393-25</t>
+          <t>EU-SVA-123456-25</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Gamma Development</t>
+          <t>STV</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>7 ks</t>
+          <t>10 ks</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -899,17 +887,17 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Test položka 1 | hovno</t>
+          <t>cavity 2 | ttttttttttt</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Petr Dvořák</t>
+          <t>Cibulka</t>
         </is>
       </c>
     </row>
@@ -921,63 +909,133 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>14:34:25</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>cibul</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Položka</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>23</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Prototyp</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>EU-SVA-761393-25</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Gamma Development</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>7 ks</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Expirace</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Test položka 1 | hovno</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>2024-08-01</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Petr Dvořák</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>13:54:37</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>cibul</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Položka</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="E9" t="n">
         <v>1</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Test díl</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>EU-SVA-123456-25</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Test Projekt</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>10 ks</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>2026-07-27</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>Chyba/Špatně zaskladněno</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>Test položka | Test archivace</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>2025-07-27</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>Updated Test User</t>
         </is>

</xml_diff>

<commit_message>
Phase 5 ČÁSTEČNĚ DOKONČENA: Header tab system + Expiry overview
✅ IMPLEMENTOVÁNO:
- Expiry overview s 7/14/30-day filtry v sidebaru
- Navigace z expirujících položek do konkrétní GB pozice
- Přeuspořádání sidebaru - expiry pod kritické sekce
- Header tab system - záložky přesunuty do hlavičky
- UI optimalizace pro maximální prostor aplikace
- CSS třídy .tab-button-header s dark mode podporou
- JavaScript integrace nových CSS selektorů

🔧 TECHNICKÉ ZMĚNY:
- backend/static/index.html: Major layout restructure - header tabs
- backend/static/css/style.css: Nové CSS třídy pro header tabs
- backend/static/js/app.js: Aktualizované selektory pro nový tab system
- backend/static/js/regaly.js: Expiry funkcionalita s filtry
- PROJECT_PLAN.md: Aktualizace Phase 5 dokumentace

⚠️ PŘESKOČENO: Komplexní analytics (na uživatelské přání)
🎯 DALŠÍ: Phase 7 - Export aktuálních dat do PDF/Excel
</commit_message>
<xml_diff>
--- a/backend/docs/vyskladneno_archiv.xlsx
+++ b/backend/docs/vyskladneno_archiv.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,7 +529,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10:56:20</t>
+          <t>12:16:42</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -539,55 +539,63 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Celý_GB</t>
+          <t>Položka</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>KOMPLETNÍ GB #7</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+          <t>sedák</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>EU-SVA-999999-25</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>BL5</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0 položek</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
+          <t>2 ks</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Chyba/Špatně zaskladněno</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>........... | blbě zadaná data</t>
-        </is>
-      </c>
+          <t>Expirace</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-08-06</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>CCCCCCCC</t>
+          <t>Cibulka</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-08-06</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14:44:36</t>
+          <t>10:56:20</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -601,29 +609,29 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>KOMPLETNÍ GB #23</t>
+          <t>KOMPLETNÍ GB #7</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2 položek</t>
+          <t>0 položek</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Rozbito/Poškozeno</t>
+          <t>Chyba/Špatně zaskladněno</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Částečně naplněný GB - kritická expirace! | uvolňuji místo, díly není třeba</t>
+          <t>........... | blbě zadaná data</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -633,7 +641,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Petr Dvořák</t>
+          <t>CCCCCCCC</t>
         </is>
       </c>
     </row>
@@ -655,7 +663,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Položka_z_GB</t>
+          <t>Celý_GB</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -663,38 +671,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Mechanický díl</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>EU-SVA-156707-25</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Projekt Alpha</t>
-        </is>
-      </c>
+          <t>KOMPLETNÍ GB #23</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>13 ks</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>2026-05-14</t>
-        </is>
-      </c>
+          <t>2 položek</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
           <t>Rozbito/Poškozeno</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Částečně naplněný GB - kritická expirace! | uvolňuji místo, díly není třeba</t>
+        </is>
+      </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2025-05-14</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -729,12 +729,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Elektronická část</t>
+          <t>Mechanický díl</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>EU-SVA-471870-25</t>
+          <t>EU-SVA-156707-25</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -744,12 +744,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>26 ks</t>
+          <t>13 ks</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-05-14</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -757,14 +757,10 @@
           <t>Rozbito/Poškozeno</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Test položka 3</t>
-        </is>
-      </c>
+      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2025-02-17</t>
+          <t>2025-05-14</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -781,7 +777,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>14:42:39</t>
+          <t>14:44:36</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -791,43 +787,55 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Celý_GB</t>
+          <t>Položka_z_GB</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>KOMPLETNÍ GB #15</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+          <t>Elektronická část</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>EU-SVA-471870-25</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Projekt Alpha</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0 položek</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
+          <t>26 ks</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Jiné</t>
+          <t>Rozbito/Poškozeno</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>....</t>
+          <t>Test položka 3</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2025-07-27</t>
+          <t>2025-02-17</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Cibulka</t>
+          <t>Petr Dvořák</t>
         </is>
       </c>
     </row>
@@ -839,7 +847,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>14:41:53</t>
+          <t>14:42:39</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -849,7 +857,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Položka</t>
+          <t>Celý_GB</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -857,42 +865,30 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>topplate</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>EU-SVA-123456-25</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>STV</t>
-        </is>
-      </c>
+          <t>KOMPLETNÍ GB #15</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>10 ks</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>2025-08-01</t>
-        </is>
-      </c>
+          <t>0 položek</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Expirace</t>
+          <t>Jiné</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>cavity 2 | ttttttttttt</t>
+          <t>....</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2025-08-02</t>
+          <t>2025-07-27</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -909,7 +905,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>14:34:25</t>
+          <t>14:41:53</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -923,26 +919,26 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Prototyp</t>
+          <t>topplate</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>EU-SVA-761393-25</t>
+          <t>EU-SVA-123456-25</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Gamma Development</t>
+          <t>STV</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>7 ks</t>
+          <t>10 ks</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -957,17 +953,17 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Test položka 1 | hovno</t>
+          <t>cavity 2 | ttttttttttt</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2025-08-02</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Petr Dvořák</t>
+          <t>Cibulka</t>
         </is>
       </c>
     </row>
@@ -979,63 +975,133 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>14:34:25</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>cibul</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Položka</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>23</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Prototyp</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>EU-SVA-761393-25</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Gamma Development</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>7 ks</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Expirace</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Test položka 1 | hovno</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>2024-08-01</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Petr Dvořák</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-08-02</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>13:54:37</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>cibul</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Položka</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>1</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Test díl</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>EU-SVA-123456-25</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>Test Projekt</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>10 ks</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>2026-07-27</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>Chyba/Špatně zaskladněno</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>Test položka | Test archivace</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>2025-07-27</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>Updated Test User</t>
         </is>

</xml_diff>